<commit_message>
Nearly ready for submission. Just need to go over the problems and write a part intro for the first bit.
</commit_message>
<xml_diff>
--- a/s_Posterior_PS_googleSearchIntervals.xlsx
+++ b/s_Posterior_PS_googleSearchIntervals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="19">
   <si>
     <t>Starting</t>
   </si>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N7"/>
+  <dimension ref="B2:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,6 +1190,38 @@
         <v>0.33000000000000007</v>
       </c>
     </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+      <c r="J9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>